<commit_message>
Fixed problem with not displaying first match of each team
finished for beach blitz data
</commit_message>
<xml_diff>
--- a/LATeamDataTest8.xlsx
+++ b/LATeamDataTest8.xlsx
@@ -59,8 +59,6 @@
     <sheet name="6668" sheetId="50" state="visible" r:id="rId50"/>
     <sheet name="6833" sheetId="51" state="visible" r:id="rId51"/>
     <sheet name="6915" sheetId="52" state="visible" r:id="rId52"/>
-    <sheet name="6938" sheetId="53" state="visible" r:id="rId53"/>
-    <sheet name="7042" sheetId="54" state="visible" r:id="rId54"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -478,7 +476,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G54"/>
+  <dimension ref="A1:G52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1662,52 +1660,6 @@
       </c>
       <c r="G52" t="n">
         <v>8.4</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7">
-      <c r="A53" t="n">
-        <v>6915</v>
-      </c>
-      <c r="B53" t="n">
-        <v>0</v>
-      </c>
-      <c r="C53" t="n">
-        <v>0</v>
-      </c>
-      <c r="D53" t="n">
-        <v>0</v>
-      </c>
-      <c r="E53" t="n">
-        <v>0</v>
-      </c>
-      <c r="F53" t="n">
-        <v>0</v>
-      </c>
-      <c r="G53" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7">
-      <c r="A54" t="n">
-        <v>6938</v>
-      </c>
-      <c r="B54" t="n">
-        <v>0</v>
-      </c>
-      <c r="C54" t="n">
-        <v>0</v>
-      </c>
-      <c r="D54" t="n">
-        <v>0</v>
-      </c>
-      <c r="E54" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="F54" t="n">
-        <v>0</v>
-      </c>
-      <c r="G54" t="n">
-        <v>0.48</v>
       </c>
     </row>
   </sheetData>
@@ -14972,628 +14924,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K26"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" t="n">
-        <v>6</v>
-      </c>
-      <c r="E1" t="n">
-        <v>6915</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" t="n">
-        <v>54</v>
-      </c>
-      <c r="B4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" t="n">
-        <v>5</v>
-      </c>
-      <c r="B5" t="n">
-        <v>0</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6" t="n">
-        <v>15</v>
-      </c>
-      <c r="B6" t="n">
-        <v>0</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="A7" t="n">
-        <v>21</v>
-      </c>
-      <c r="B7" t="n">
-        <v>0</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="A8" t="n">
-        <v>28</v>
-      </c>
-      <c r="B8" t="n">
-        <v>0</v>
-      </c>
-      <c r="C8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="A9" t="n">
-        <v>41</v>
-      </c>
-      <c r="B9" t="n">
-        <v>0</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11">
-      <c r="B19" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11">
-      <c r="A20" t="s">
-        <v>9</v>
-      </c>
-      <c r="B20" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" t="s">
-        <v>17</v>
-      </c>
-      <c r="D20" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20" t="s">
-        <v>12</v>
-      </c>
-      <c r="F20" t="s">
-        <v>18</v>
-      </c>
-      <c r="G20" t="s">
-        <v>19</v>
-      </c>
-      <c r="I20" t="s">
-        <v>14</v>
-      </c>
-      <c r="J20" t="s">
-        <v>20</v>
-      </c>
-      <c r="K20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11">
-      <c r="A21" t="n">
-        <v>11</v>
-      </c>
-      <c r="B21" t="n">
-        <v>0</v>
-      </c>
-      <c r="C21" t="n">
-        <v>0</v>
-      </c>
-      <c r="D21" t="n">
-        <v>0</v>
-      </c>
-      <c r="E21" t="n">
-        <v>0</v>
-      </c>
-      <c r="F21" t="s">
-        <v>21</v>
-      </c>
-      <c r="G21" t="s">
-        <v>22</v>
-      </c>
-      <c r="I21" t="n">
-        <v>0</v>
-      </c>
-      <c r="J21" t="n">
-        <v>0</v>
-      </c>
-      <c r="K21" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11">
-      <c r="A22" t="n">
-        <v>22</v>
-      </c>
-      <c r="B22" t="n">
-        <v>0</v>
-      </c>
-      <c r="C22" t="n">
-        <v>0</v>
-      </c>
-      <c r="D22" t="n">
-        <v>0</v>
-      </c>
-      <c r="E22" t="n">
-        <v>0</v>
-      </c>
-      <c r="F22" t="s">
-        <v>21</v>
-      </c>
-      <c r="G22" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11">
-      <c r="A23" t="n">
-        <v>36</v>
-      </c>
-      <c r="B23" t="n">
-        <v>0</v>
-      </c>
-      <c r="C23" t="n">
-        <v>0</v>
-      </c>
-      <c r="D23" t="n">
-        <v>0</v>
-      </c>
-      <c r="E23" t="n">
-        <v>0</v>
-      </c>
-      <c r="F23" t="s">
-        <v>21</v>
-      </c>
-      <c r="G23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11">
-      <c r="A24" t="n">
-        <v>44</v>
-      </c>
-      <c r="B24" t="n">
-        <v>0</v>
-      </c>
-      <c r="C24" t="n">
-        <v>0</v>
-      </c>
-      <c r="D24" t="n">
-        <v>0</v>
-      </c>
-      <c r="E24" t="n">
-        <v>0</v>
-      </c>
-      <c r="F24" t="s">
-        <v>21</v>
-      </c>
-      <c r="G24" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11">
-      <c r="A25" t="n">
-        <v>50</v>
-      </c>
-      <c r="B25" t="n">
-        <v>0</v>
-      </c>
-      <c r="C25" t="n">
-        <v>0</v>
-      </c>
-      <c r="D25" t="n">
-        <v>0</v>
-      </c>
-      <c r="E25" t="n">
-        <v>0</v>
-      </c>
-      <c r="F25" t="s">
-        <v>21</v>
-      </c>
-      <c r="G25" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11">
-      <c r="A26" t="n">
-        <v>57</v>
-      </c>
-      <c r="B26" t="n">
-        <v>0</v>
-      </c>
-      <c r="C26" t="n">
-        <v>0</v>
-      </c>
-      <c r="D26" t="n">
-        <v>0</v>
-      </c>
-      <c r="E26" t="n">
-        <v>0</v>
-      </c>
-      <c r="F26" t="s">
-        <v>21</v>
-      </c>
-      <c r="G26" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:K25"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" t="n">
-        <v>5</v>
-      </c>
-      <c r="E1" t="n">
-        <v>6938</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" t="n">
-        <v>7</v>
-      </c>
-      <c r="B4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" t="n">
-        <v>12</v>
-      </c>
-      <c r="B5" t="n">
-        <v>0</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6" t="n">
-        <v>35</v>
-      </c>
-      <c r="B6" t="n">
-        <v>0</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="A7" t="n">
-        <v>41</v>
-      </c>
-      <c r="B7" t="n">
-        <v>0</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="A8" t="n">
-        <v>50</v>
-      </c>
-      <c r="B8" t="n">
-        <v>0</v>
-      </c>
-      <c r="C8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11">
-      <c r="B19" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11">
-      <c r="A20" t="s">
-        <v>9</v>
-      </c>
-      <c r="B20" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" t="s">
-        <v>17</v>
-      </c>
-      <c r="D20" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20" t="s">
-        <v>12</v>
-      </c>
-      <c r="F20" t="s">
-        <v>18</v>
-      </c>
-      <c r="G20" t="s">
-        <v>19</v>
-      </c>
-      <c r="I20" t="s">
-        <v>14</v>
-      </c>
-      <c r="J20" t="s">
-        <v>20</v>
-      </c>
-      <c r="K20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11">
-      <c r="A21" t="n">
-        <v>10</v>
-      </c>
-      <c r="B21" t="n">
-        <v>0</v>
-      </c>
-      <c r="C21" t="n">
-        <v>2</v>
-      </c>
-      <c r="D21" t="n">
-        <v>0</v>
-      </c>
-      <c r="E21" t="n">
-        <v>2</v>
-      </c>
-      <c r="F21" t="s">
-        <v>21</v>
-      </c>
-      <c r="G21" t="s">
-        <v>22</v>
-      </c>
-      <c r="I21" t="n">
-        <v>0</v>
-      </c>
-      <c r="J21" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="K21" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11">
-      <c r="A22" t="n">
-        <v>20</v>
-      </c>
-      <c r="B22" t="n">
-        <v>0</v>
-      </c>
-      <c r="C22" t="n">
-        <v>0</v>
-      </c>
-      <c r="D22" t="n">
-        <v>0</v>
-      </c>
-      <c r="E22" t="n">
-        <v>0</v>
-      </c>
-      <c r="F22" t="s">
-        <v>21</v>
-      </c>
-      <c r="G22" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11">
-      <c r="A23" t="n">
-        <v>31</v>
-      </c>
-      <c r="B23" t="n">
-        <v>0</v>
-      </c>
-      <c r="C23" t="n">
-        <v>0</v>
-      </c>
-      <c r="D23" t="n">
-        <v>0</v>
-      </c>
-      <c r="E23" t="n">
-        <v>0</v>
-      </c>
-      <c r="F23" t="s">
-        <v>21</v>
-      </c>
-      <c r="G23" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11">
-      <c r="A24" t="n">
-        <v>43</v>
-      </c>
-      <c r="B24" t="n">
-        <v>0</v>
-      </c>
-      <c r="C24" t="n">
-        <v>0</v>
-      </c>
-      <c r="D24" t="n">
-        <v>0</v>
-      </c>
-      <c r="E24" t="n">
-        <v>0</v>
-      </c>
-      <c r="F24" t="s">
-        <v>21</v>
-      </c>
-      <c r="G24" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11">
-      <c r="A25" t="n">
-        <v>54</v>
-      </c>
-      <c r="B25" t="n">
-        <v>0</v>
-      </c>
-      <c r="C25" t="n">
-        <v>0</v>
-      </c>
-      <c r="D25" t="n">
-        <v>0</v>
-      </c>
-      <c r="E25" t="n">
-        <v>0</v>
-      </c>
-      <c r="F25" t="s">
-        <v>21</v>
-      </c>
-      <c r="G25" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15603,7 +14934,7 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="E1" t="n">
-        <v>7042</v>
+        <v>6915</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -15636,7 +14967,7 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="n">
-        <v>18</v>
+        <v>54</v>
       </c>
       <c r="B4" t="n">
         <v>0</v>
@@ -15650,7 +14981,7 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="n">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="B5" t="n">
         <v>0</v>
@@ -15659,34 +14990,6 @@
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6" t="n">
-        <v>31</v>
-      </c>
-      <c r="B6" t="n">
-        <v>0</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="A7" t="n">
-        <v>39</v>
-      </c>
-      <c r="B7" t="n">
-        <v>0</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -15729,33 +15032,33 @@
     </row>
     <row r="21" spans="1:11">
       <c r="A21" t="n">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D21" t="n">
         <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F21" t="s">
         <v>21</v>
       </c>
       <c r="G21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:11">
       <c r="A22" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
@@ -15764,59 +15067,13 @@
         <v>0</v>
       </c>
       <c r="E22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F22" t="s">
         <v>21</v>
       </c>
       <c r="G22" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11">
-      <c r="A23" t="n">
-        <v>28</v>
-      </c>
-      <c r="B23" t="n">
-        <v>1</v>
-      </c>
-      <c r="C23" t="n">
-        <v>0</v>
-      </c>
-      <c r="D23" t="n">
-        <v>0</v>
-      </c>
-      <c r="E23" t="n">
-        <v>1</v>
-      </c>
-      <c r="F23" t="s">
-        <v>21</v>
-      </c>
-      <c r="G23" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11">
-      <c r="A24" t="n">
-        <v>41</v>
-      </c>
-      <c r="B24" t="n">
-        <v>0</v>
-      </c>
-      <c r="C24" t="n">
-        <v>3</v>
-      </c>
-      <c r="D24" t="n">
-        <v>0</v>
-      </c>
-      <c r="E24" t="n">
-        <v>3</v>
-      </c>
-      <c r="F24" t="s">
-        <v>21</v>
-      </c>
-      <c r="G24" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>